<commit_message>
Adição de tempo de preparo na receita
</commit_message>
<xml_diff>
--- a/server/src/util/util/excel/modelo-receita.xlsx
+++ b/server/src/util/util/excel/modelo-receita.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\andrevpk\TADS\6ºPeríodo\TCC_II\RandomFoods\backend\src\database\imports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C6730AA-5F31-4A41-9E1A-B225B09EC2CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3329F24-2306-4206-94EA-7DF358E0AD98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Receita" sheetId="1" r:id="rId1"/>
     <sheet name="Ingrediente" sheetId="2" r:id="rId2"/>
     <sheet name="Categoria" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,12 +36,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>nome</t>
   </si>
   <si>
     <t>descricao</t>
+  </si>
+  <si>
+    <t>tempoPreparo</t>
   </si>
   <si>
     <t>tipo</t>
@@ -106,9 +109,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -425,36 +427,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView zoomScale="147" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.15"/>
   <cols>
     <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="D2" s="2"/>
+    <row r="2" spans="1:5">
+      <c r="E2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -468,7 +474,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
@@ -476,105 +482,25 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.15"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4"/>
-      <c r="B4"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="D16" s="1"/>
-    </row>
-    <row r="19" spans="4:4">
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="4:4">
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="4:4">
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="4:4">
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="4:4">
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="4:4">
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="4:4">
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="4:4">
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="4:4">
-      <c r="D27" s="1"/>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -588,38 +514,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.15"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="B6" s="1"/>
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>